<commit_message>
fix array compatibility in 2k19
</commit_message>
<xml_diff>
--- a/_ToDo/Scoring Matrix.xlsx
+++ b/_ToDo/Scoring Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loicveirman/Documents/GitHub/Pimp-My-Directory/_ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28550797-4DD2-C34C-B469-4FD48B1AF0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D19869F-46E6-3B45-8DC7-434F6D76D04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="540" windowWidth="25320" windowHeight="28220" xr2:uid="{65454DCD-A632-5C41-82AD-606BA14167F1}"/>
+    <workbookView xWindow="26380" yWindow="540" windowWidth="50640" windowHeight="28220" xr2:uid="{65454DCD-A632-5C41-82AD-606BA14167F1}"/>
   </bookViews>
   <sheets>
     <sheet name="HmD 1.0.0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>SCORING MATRIX</t>
   </si>
@@ -87,18 +87,46 @@
   </si>
   <si>
     <t>Notes:</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Advise Sol.</t>
+  </si>
+  <si>
+    <t>WinSrv 2019 en</t>
+  </si>
+  <si>
+    <t>Alert Fix List</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>P-Delegated</t>
+  </si>
+  <si>
+    <t>A-MinPwdLen</t>
+  </si>
+  <si>
+    <t>Could not be done through a cmdlet. Find an alternative.</t>
+  </si>
+  <si>
+    <t>Check code, seems to work only on 2022. Works on second run.</t>
   </si>
   <si>
     <t>PingCastle compute a risk exposure (target: 0%).
 The Forest is raised to its highest FFL.
-The test Domain contain two DC.</t>
+The test Domain contain two DC.
+Windows 2012 R2 needs to be updated to PowserShell 5.0, else the modules will fail to load.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -146,6 +174,11 @@
       <sz val="14"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Poppins-Light"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Poppins-Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -390,7 +423,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
@@ -493,6 +526,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -513,6 +564,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74A0EFC9-44C1-8542-A79B-ABEE2E27F50F}" name="Tableau1" displayName="Tableau1" ref="R5:U7" totalsRowShown="0">
+  <autoFilter ref="R5:U7" xr:uid="{74A0EFC9-44C1-8542-A79B-ABEE2E27F50F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{618D3CCF-1CED-7C4A-8418-5829ED2B56C9}" name="OS"/>
+    <tableColumn id="2" xr3:uid="{D6659A65-2B54-2349-842B-34CA3657B08B}" name="DFL"/>
+    <tableColumn id="3" xr3:uid="{492BE08A-F01D-9345-8055-76B3C5D00BF2}" name="Alert"/>
+    <tableColumn id="4" xr3:uid="{61A8E3D9-0DA4-F443-A20D-32E019DD63E8}" name="Advise Sol."/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -718,19 +782,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1518DF-B98A-CB44-9D73-BA4BD0420A53}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="J9" sqref="J9:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
   <cols>
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="11" width="7.77734375" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="19" max="19" width="11.77734375" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" customWidth="1"/>
+    <col min="21" max="21" width="62.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" thickBot="1">
+    <row r="1" spans="1:21" ht="30" thickBot="1">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -745,8 +813,8 @@
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
     </row>
-    <row r="2" spans="1:16" ht="23" thickTop="1"/>
-    <row r="3" spans="1:16">
+    <row r="2" spans="1:21" ht="23" thickTop="1"/>
+    <row r="3" spans="1:21">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -755,12 +823,15 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:21">
       <c r="M4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="R4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
@@ -785,13 +856,25 @@
       </c>
       <c r="K5" s="21"/>
       <c r="M5" s="23" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="N5" s="23"/>
       <c r="O5" s="23"/>
       <c r="P5" s="23"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="R5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -827,8 +910,20 @@
       <c r="N6" s="23"/>
       <c r="O6" s="23"/>
       <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="R6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
@@ -846,8 +941,20 @@
       <c r="N7" s="23"/>
       <c r="O7" s="23"/>
       <c r="P7" s="23"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="R7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" t="s">
+        <v>6</v>
+      </c>
+      <c r="T7" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -857,7 +964,9 @@
         <v>0</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="9">
+        <v>0.2</v>
+      </c>
       <c r="G8" s="11"/>
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
@@ -868,7 +977,7 @@
       <c r="O8" s="23"/>
       <c r="P8" s="23"/>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:21">
       <c r="A9" s="17" t="s">
         <v>7</v>
       </c>
@@ -880,14 +989,14 @@
       <c r="G9" s="14"/>
       <c r="H9" s="12"/>
       <c r="I9" s="13"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="13"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="37"/>
       <c r="M9" s="23"/>
       <c r="N9" s="23"/>
       <c r="O9" s="23"/>
       <c r="P9" s="23"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:21">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -899,14 +1008,14 @@
       <c r="G10" s="11"/>
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="10"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
       <c r="P10" s="23"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:21">
       <c r="A11" s="15" t="s">
         <v>9</v>
       </c>
@@ -918,14 +1027,14 @@
       <c r="G11" s="8"/>
       <c r="H11" s="6"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="7"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="41"/>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
       <c r="P11" s="23"/>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:21">
       <c r="A12" s="16" t="s">
         <v>13</v>
       </c>
@@ -937,14 +1046,14 @@
       <c r="G12" s="11"/>
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="39"/>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
       <c r="O12" s="23"/>
       <c r="P12" s="23"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:21">
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
@@ -956,14 +1065,14 @@
       <c r="G13" s="8"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="7"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="41"/>
       <c r="M13" s="23"/>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
       <c r="P13" s="23"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:21">
       <c r="A14" s="16" t="s">
         <v>15</v>
       </c>
@@ -975,8 +1084,8 @@
       <c r="G14" s="11"/>
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="10"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
       <c r="M14" s="23"/>
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
@@ -994,5 +1103,8 @@
     <mergeCell ref="F5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix some minor issues.
</commit_message>
<xml_diff>
--- a/_ToDo/Scoring Matrix.xlsx
+++ b/_ToDo/Scoring Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loicveirman/Documents/GitHub/Pimp-My-Directory/_ToDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D19869F-46E6-3B45-8DC7-434F6D76D04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99A4455-9B33-154E-BBBE-75300CC8EF78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26380" yWindow="540" windowWidth="50640" windowHeight="28220" xr2:uid="{65454DCD-A632-5C41-82AD-606BA14167F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>SCORING MATRIX</t>
   </si>
@@ -114,19 +114,43 @@
   </si>
   <si>
     <t>Check code, seems to work only on 2022. Works on second run.</t>
+  </si>
+  <si>
+    <t>KO</t>
   </si>
   <si>
     <t>PingCastle compute a risk exposure (target: 0%).
 The Forest is raised to its highest FFL.
 The test Domain contain two DC.
 Windows 2012 R2 needs to be updated to PowserShell 5.0, else the modules will fail to load.</t>
+  </si>
+  <si>
+    <t>WinSrv 2016 en</t>
+  </si>
+  <si>
+    <t>S-SMB-v1</t>
+  </si>
+  <si>
+    <t>SMBv1 have to be disabled forcefully.</t>
+  </si>
+  <si>
+    <t>S-DC-SubnetMissing</t>
+  </si>
+  <si>
+    <t>IPv6 subnet are not yet added… This concern all OS ;)</t>
+  </si>
+  <si>
+    <t>A-LAPS-Not-Installed</t>
+  </si>
+  <si>
+    <t>LAPS installation has failed (error on screen)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -176,7 +200,26 @@
       <name val="Poppins-Light"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
+      <color rgb="FF00B050"/>
+      <name val="Poppins-Light"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Poppins-Light"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Poppins-Light"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Poppins-Light"/>
       <family val="2"/>
     </font>
@@ -423,7 +466,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
@@ -438,33 +481,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -528,24 +544,55 @@
     <xf numFmtId="9" fontId="0" fillId="8" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calcul" xfId="3" builtinId="22"/>
@@ -567,8 +614,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74A0EFC9-44C1-8542-A79B-ABEE2E27F50F}" name="Tableau1" displayName="Tableau1" ref="R5:U7" totalsRowShown="0">
-  <autoFilter ref="R5:U7" xr:uid="{74A0EFC9-44C1-8542-A79B-ABEE2E27F50F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74A0EFC9-44C1-8542-A79B-ABEE2E27F50F}" name="Tableau1" displayName="Tableau1" ref="R5:U11" totalsRowShown="0">
+  <autoFilter ref="R5:U11" xr:uid="{74A0EFC9-44C1-8542-A79B-ABEE2E27F50F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{618D3CCF-1CED-7C4A-8418-5829ED2B56C9}" name="OS"/>
     <tableColumn id="2" xr3:uid="{D6659A65-2B54-2349-842B-34CA3657B08B}" name="DFL"/>
@@ -785,7 +832,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:K14"/>
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22"/>
@@ -799,19 +846,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30" thickBot="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:21" ht="23" thickTop="1"/>
     <row r="3" spans="1:21">
@@ -832,35 +879,35 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="24" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="20" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="20" t="s">
+      <c r="I5" s="12"/>
+      <c r="J5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="M5" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
+      <c r="K5" s="12"/>
+      <c r="M5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
       <c r="R5" t="s">
         <v>17</v>
       </c>
@@ -875,7 +922,7 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="19"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -906,41 +953,41 @@
       <c r="K6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="R6" t="s">
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="R6" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="U6" t="s">
+      <c r="U6" s="43" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="32"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
       <c r="R7" t="s">
         <v>19</v>
       </c>
@@ -955,141 +1002,213 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="9">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="27">
         <v>0</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="R8" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8" t="s">
+        <v>23</v>
+      </c>
+      <c r="U8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="37"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="R9" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="S9" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="T9" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="U9" s="43" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="R10" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" t="s">
+        <v>31</v>
+      </c>
+      <c r="U10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="41"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="R11" t="s">
+        <v>28</v>
+      </c>
+      <c r="S11" t="s">
+        <v>6</v>
+      </c>
+      <c r="T11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="39"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>